<commit_message>
Added data for inventory log
</commit_message>
<xml_diff>
--- a/MissIssippiDB/0 Database/MissIssippiDB schema.xlsx
+++ b/MissIssippiDB/0 Database/MissIssippiDB schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silky\source\repos\Miss Issippi Software\MissIssippiDB\0 Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51F4428-6C72-4D98-A81E-EE3A624E9DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC53C60-F079-4456-9A92-7B35C56DDDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{D68B08DA-DC10-4AE7-AB5A-98819CC89915}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>Sizes</t>
   </si>
@@ -210,9 +210,6 @@
     <t>varchar500</t>
   </si>
   <si>
-    <t>InStock</t>
-  </si>
-  <si>
     <t>SizeSequence</t>
   </si>
   <si>
@@ -241,6 +238,12 @@
   </si>
   <si>
     <t>InventoryActivityDate</t>
+  </si>
+  <si>
+    <t>;wi</t>
+  </si>
+  <si>
+    <t>InStock - commented out</t>
   </si>
 </sst>
 </file>
@@ -289,7 +292,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +358,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -441,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -484,6 +493,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -801,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C16E8A-B658-4CBD-9CE4-054BA3F59930}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
@@ -893,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -976,7 +986,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>24</v>
@@ -1045,7 +1055,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="K14" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
@@ -1067,7 +1077,7 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="K15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>38</v>
@@ -1079,10 +1089,10 @@
         <v>46</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="20" t="s">
         <v>67</v>
-      </c>
-      <c r="P15" s="20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1099,7 +1109,7 @@
         <v>45</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>1</v>
@@ -1107,8 +1117,8 @@
       <c r="H16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>58</v>
+      <c r="I16" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>3</v>
@@ -1123,10 +1133,10 @@
         <v>47</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1151,7 +1161,7 @@
       <c r="H17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1177,7 +1187,7 @@
         <v>52</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>